<commit_message>
combine genomic traits and experiments into one big table
</commit_message>
<xml_diff>
--- a/genomic_traits/experimental assays/10cc ROS and proteolytic result.xlsx
+++ b/genomic_traits/experimental assays/10cc ROS and proteolytic result.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Osnat\Documents\GitHub\recycle_model\genomic_traits\experimental assays\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oweisberg\Documents\GitHub\recycle_model\genomic_traits\experimental assays\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB9E5A19-B703-4677-80B0-617AA6E238D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{977D5A73-03D9-44B4-B3E2-F98A106A6ECB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3615" yWindow="3120" windowWidth="21600" windowHeight="12645" activeTab="1" xr2:uid="{600B41F4-FE38-448B-99BD-C3EB69F0B780}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{600B41F4-FE38-448B-99BD-C3EB69F0B780}"/>
   </bookViews>
   <sheets>
     <sheet name="ROS detoxification" sheetId="1" r:id="rId1"/>
@@ -254,10 +254,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -915,10 +915,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0A8A168-C48E-4507-B9CC-323A1683FC42}">
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -983,22 +983,22 @@
         <v>31</v>
       </c>
       <c r="D3" s="2">
-        <v>-8.5192687931107575E-8</v>
+        <v>-8.5192687931107569E-2</v>
       </c>
       <c r="E3" s="2">
-        <v>-6.2940267139812723E-8</v>
+        <v>-6.2940267139812725E-2</v>
       </c>
       <c r="F3" s="2">
-        <v>8.5192687931107575E-8</v>
+        <v>8.5192687931107569E-2</v>
       </c>
       <c r="G3" s="2">
-        <v>6.2940267139812723E-8</v>
+        <v>6.2940267139812725E-2</v>
       </c>
       <c r="H3" s="2">
-        <v>7.4066477535460142E-8</v>
-      </c>
-      <c r="I3" s="1">
-        <v>1.573483763934111E-8</v>
+        <v>7.406647753546014E-2</v>
+      </c>
+      <c r="I3" s="2">
+        <v>1.5734837639341109E-2</v>
       </c>
       <c r="J3" s="3">
         <v>0.2124420947628822</v>
@@ -1022,22 +1022,22 @@
         <v>31</v>
       </c>
       <c r="D4" s="2">
-        <v>-7.0229028856940819E-8</v>
+        <v>-7.0229028856940823E-2</v>
       </c>
       <c r="E4" s="2">
-        <v>-4.9641699465750472E-8</v>
+        <v>-4.964169946575047E-2</v>
       </c>
       <c r="F4" s="2">
-        <v>7.0229028856940819E-8</v>
+        <v>7.0229028856940823E-2</v>
       </c>
       <c r="G4" s="2">
-        <v>4.9641699465750472E-8</v>
+        <v>4.964169946575047E-2</v>
       </c>
       <c r="H4" s="2">
-        <v>5.9935364161345652E-8</v>
-      </c>
-      <c r="I4" s="1">
-        <v>1.4557440219031812E-8</v>
+        <v>5.993536416134565E-2</v>
+      </c>
+      <c r="I4" s="2">
+        <v>1.4557440219031811E-2</v>
       </c>
       <c r="J4" s="3">
         <v>0.24288565561799655</v>
@@ -1061,22 +1061,22 @@
         <v>31</v>
       </c>
       <c r="D5" s="2">
-        <v>-6.4274770035325072E-9</v>
+        <v>-6.4274770035325068E-3</v>
       </c>
       <c r="E5" s="2">
-        <v>-7.9619695963120573E-9</v>
+        <v>-7.9619695963120581E-3</v>
       </c>
       <c r="F5" s="2">
-        <v>6.4274770035325072E-9</v>
+        <v>6.4274770035325068E-3</v>
       </c>
       <c r="G5" s="2">
-        <v>7.9619695963120573E-9</v>
+        <v>7.9619695963120581E-3</v>
       </c>
       <c r="H5" s="2">
-        <v>7.1947232999222818E-9</v>
-      </c>
-      <c r="I5" s="1">
-        <v>1.0850501180349473E-9</v>
+        <v>7.1947232999222815E-3</v>
+      </c>
+      <c r="I5" s="2">
+        <v>1.0850501180349472E-3</v>
       </c>
       <c r="J5" s="3">
         <v>0.15081193157861514</v>
@@ -1100,22 +1100,22 @@
         <v>31</v>
       </c>
       <c r="D6" s="2">
-        <v>-1.0570441895019552E-8</v>
+        <v>-1.0570441895019551E-2</v>
       </c>
       <c r="E6" s="5">
-        <v>-8.9414340604347451E-9</v>
+        <v>-8.9414340604347456E-3</v>
       </c>
       <c r="F6" s="2">
-        <v>1.0570441895019552E-8</v>
+        <v>1.0570441895019551E-2</v>
       </c>
       <c r="G6" s="5">
-        <v>8.9414340604347451E-9</v>
+        <v>8.9414340604347456E-3</v>
       </c>
       <c r="H6" s="5">
-        <v>9.7559379777271478E-9</v>
-      </c>
-      <c r="I6" s="6">
-        <v>1.1518824864409308E-9</v>
+        <v>9.7559379777271485E-3</v>
+      </c>
+      <c r="I6" s="5">
+        <v>1.1518824864409308E-3</v>
       </c>
       <c r="J6" s="7">
         <v>0.1180698861627333</v>
@@ -1141,22 +1141,22 @@
         <v>31</v>
       </c>
       <c r="D7" s="2">
-        <v>-2.8712170191350679E-8</v>
+        <v>-2.871217019135068E-2</v>
       </c>
       <c r="E7" s="5">
-        <v>-2.3353530609610592E-8</v>
+        <v>-2.3353530609610592E-2</v>
       </c>
       <c r="F7" s="2">
-        <v>2.8712170191350679E-8</v>
+        <v>2.871217019135068E-2</v>
       </c>
       <c r="G7" s="5">
-        <v>2.3353530609610592E-8</v>
+        <v>2.3353530609610592E-2</v>
       </c>
       <c r="H7" s="5">
-        <v>2.6032850400480636E-8</v>
-      </c>
-      <c r="I7" s="6">
-        <v>3.7891303861830599E-9</v>
+        <v>2.6032850400480635E-2</v>
+      </c>
+      <c r="I7" s="5">
+        <v>3.7891303861830599E-3</v>
       </c>
       <c r="J7" s="7">
         <v>0.14555188263645161</v>
@@ -1182,22 +1182,22 @@
         <v>31</v>
       </c>
       <c r="D8" s="5">
-        <v>-3.5323825787579214E-9</v>
+        <v>-3.5323825787579215E-3</v>
       </c>
       <c r="E8" s="2">
-        <v>-8.2692462968740715E-9</v>
+        <v>-8.2692462968740714E-3</v>
       </c>
       <c r="F8" s="5">
-        <v>8.2692462968740715E-9</v>
+        <v>8.2692462968740714E-3</v>
       </c>
       <c r="G8" s="2">
-        <v>8.2692462968740715E-9</v>
+        <v>8.2692462968740714E-3</v>
       </c>
       <c r="H8" s="5">
-        <v>5.9008144378159966E-9</v>
-      </c>
-      <c r="I8" s="6">
-        <v>3.3494684566364526E-9</v>
+        <v>5.9008144378159969E-3</v>
+      </c>
+      <c r="I8" s="5">
+        <v>3.3494684566364526E-3</v>
       </c>
       <c r="J8" s="3">
         <v>7.7822625387486494E-2</v>
@@ -1223,22 +1223,22 @@
         <v>31</v>
       </c>
       <c r="D9" s="2">
-        <v>-1.4798104630862753E-7</v>
+        <v>-0.14798104630862755</v>
       </c>
       <c r="E9" s="2">
-        <v>-1.7260917492015836E-7</v>
+        <v>-0.17260917492015837</v>
       </c>
       <c r="F9" s="2">
-        <v>1.4798104630862753E-7</v>
+        <v>0.14798104630862755</v>
       </c>
       <c r="G9" s="2">
-        <v>1.7260917492015836E-7</v>
+        <v>0.17260917492015837</v>
       </c>
       <c r="H9" s="2">
-        <v>1.6029511061439294E-7</v>
-      </c>
-      <c r="I9" s="1">
-        <v>1.7414716749147881E-8</v>
+        <v>0.16029511061439294</v>
+      </c>
+      <c r="I9" s="2">
+        <v>1.7414716749147879E-2</v>
       </c>
       <c r="J9" s="3">
         <v>0.10864159663011087</v>
@@ -1262,24 +1262,24 @@
         <v>31</v>
       </c>
       <c r="D10" s="8">
-        <v>-9.4483272951446183E-9</v>
+        <v>-9.4483272951446182E-3</v>
       </c>
       <c r="E10" s="8">
-        <v>-9.4570493031161489E-9</v>
+        <v>-9.4570493031161489E-3</v>
       </c>
       <c r="F10" s="8">
-        <v>9.4483272951446183E-9</v>
+        <v>9.4483272951446182E-3</v>
       </c>
       <c r="G10" s="8">
-        <v>9.4570493031161489E-9</v>
+        <v>9.4570493031161489E-3</v>
       </c>
       <c r="H10" s="8">
-        <v>9.4526882991303836E-9</v>
-      </c>
-      <c r="I10" s="9">
-        <v>6.1673909822324345E-12</v>
-      </c>
-      <c r="J10" s="10">
+        <v>9.4526882991303844E-3</v>
+      </c>
+      <c r="I10" s="8">
+        <v>6.1673909822324344E-6</v>
+      </c>
+      <c r="J10" s="9">
         <v>6.5244836040979101E-4</v>
       </c>
       <c r="K10" s="4">
@@ -1289,6 +1289,86 @@
         <v>6.1673909822324344E-6</v>
       </c>
       <c r="M10" s="1"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+    </row>
+    <row r="17" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+    </row>
+    <row r="18" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+    </row>
+    <row r="19" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+    </row>
+    <row r="20" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+    </row>
+    <row r="21" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+    </row>
+    <row r="22" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1299,7 +1379,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EBC9D7F-EE03-43BA-87A6-5D65F3CE7940}">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -1311,38 +1391,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="10" t="s">
         <v>19</v>
       </c>
       <c r="B2" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="G2" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="H2" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="I2" s="10" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>